<commit_message>
add table and first couple points
</commit_message>
<xml_diff>
--- a/SOE-response-memo/2019requests.xlsx
+++ b/SOE-response-memo/2019requests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="212">
   <si>
     <t>Request</t>
   </si>
@@ -29,18 +29,18 @@
     <t>Memo Section</t>
   </si>
   <si>
+    <t>Working group</t>
+  </si>
+  <si>
+    <t>Report Section</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
     <t>Formal response to requests</t>
   </si>
   <si>
-    <t>Working group</t>
-  </si>
-  <si>
-    <t>Report Section</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
     <t>Products/ things to work on</t>
   </si>
   <si>
@@ -65,6 +65,9 @@
     <t>SOE summary bullets (page 1)</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>All</t>
   </si>
   <si>
@@ -74,79 +77,94 @@
     <t>Uncertainty estimates for all indicators</t>
   </si>
   <si>
-    <t>include summary visualization</t>
-  </si>
-  <si>
     <t>SOE survey biomass</t>
   </si>
   <si>
+    <t>Indicator specific uncertainty estimates</t>
+  </si>
+  <si>
+    <t>Include summary visualization</t>
+  </si>
+  <si>
     <t>SOE infographics (page 2)</t>
   </si>
   <si>
-    <t>Indicator specific uncertainty estimates</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Improve communciation</t>
   </si>
   <si>
     <t>Include uncertainty estimates for all indicators</t>
   </si>
   <si>
+    <t>Include Downeast ME (Scotian Shelf EPU)</t>
+  </si>
+  <si>
+    <t>NEFMC</t>
+  </si>
+  <si>
+    <t>SOE survey biomass, and many indicators include</t>
+  </si>
+  <si>
     <t>SOE survey biomass uncertainty included; feedback requested for other indicators</t>
   </si>
   <si>
-    <t>Improve communciation</t>
-  </si>
-  <si>
-    <t>Include Downeast ME (Scotian Shelf EPU)</t>
-  </si>
-  <si>
-    <t>NEFMC</t>
-  </si>
-  <si>
-    <t>SOE survey biomass, and many indicators include</t>
+    <t>3</t>
   </si>
   <si>
     <t>Ask Council/SSC</t>
   </si>
   <si>
+    <t>include as SS or combined SS and GOM? SSC comment just says to clarify, could continue with current GOM</t>
+  </si>
+  <si>
+    <t>Climate/LTL/Habitat</t>
+  </si>
+  <si>
     <t>SOE survey biomass now includes most; included in other indicators</t>
   </si>
   <si>
-    <t>include as SS or combined SS and GOM? SSC comment just says to clarify, could continue with current GOM</t>
-  </si>
-  <si>
-    <t>Climate/LTL/Habitat</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Habitat Quality and Ecosystem Productivity</t>
   </si>
   <si>
     <t>Link zooplankton abundance and or community composition to fish condition</t>
   </si>
   <si>
-    <t>Habitat Quality and Ecosystem Productivity</t>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Link zooplankton abundance and or comunity composition to fish condition</t>
   </si>
   <si>
     <t>SOE page 2 research spotlight</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Link zooplankton abundance and or comunity composition to fish condition</t>
+    <t>SOE 2 pager, explain ongoing research in memo</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Synthesize existing indicators</t>
   </si>
   <si>
     <t>Ocean acidification information</t>
   </si>
   <si>
-    <t>SOE 2 pager, explain ongoing research in memo</t>
-  </si>
-  <si>
-    <t>Synthesize existing indicators</t>
-  </si>
-  <si>
     <t>Add longline survey condition?</t>
   </si>
   <si>
+    <t>both already in this section</t>
+  </si>
+  <si>
     <t>inadequate information for indicator; existing info summarized here</t>
   </si>
   <si>
-    <t>both already in this section</t>
+    <t>6</t>
   </si>
   <si>
     <t>Gulf Stream Index/Labrador current interaction</t>
@@ -173,91 +191,166 @@
     <t>Already in report, integrate with other indicators?</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>Include source for PP estimates (satellite vs in situ)</t>
   </si>
   <si>
+    <t>SOE clarified that all PP estiamtes are from satellite</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Shellfish growth/distribution linked to climate (system productivity)</t>
+  </si>
+  <si>
+    <t>MAFMC</t>
+  </si>
+  <si>
     <t>SOE add to text satellite</t>
   </si>
   <si>
-    <t>SOE clarified that all PP estiamtes are from satellite</t>
+    <t>project with R. Mann student to start late 2020</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
   <si>
     <t>Easy, just clarify in report</t>
   </si>
   <si>
-    <t>Shellfish growth/distribution linked to climate (system productivity)</t>
-  </si>
-  <si>
-    <t>MAFMC</t>
-  </si>
-  <si>
-    <t>project with R. Mann student to start late 2020</t>
+    <t>Esturine condition relative to power plants and temp</t>
+  </si>
+  <si>
+    <t>inadequate resourses to address this year</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>Fish and Invertebrates LINK TO Habitat Quality and Ecosystem Productivity</t>
   </si>
   <si>
+    <t>Frequency and occurance of warm rings</t>
+  </si>
+  <si>
     <t>Moderate</t>
   </si>
   <si>
     <t>Shellfish growth'dist linked to climate (system productivity)</t>
   </si>
   <si>
-    <t>Esturine condition relative to power plants and temp</t>
+    <t>SOE added indicator</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
   <si>
     <t>project with R Mann student to start late 2020? in memo</t>
   </si>
   <si>
-    <t>inadequate resourses to address this year</t>
+    <t>Cold pool index</t>
   </si>
   <si>
     <t>(Roger Mann VIMS data Contribution)</t>
   </si>
   <si>
-    <t>Frequency and occurance of warm rings</t>
+    <t>12</t>
   </si>
   <si>
     <t>Economic and Social (new section Other Ocean Uses?)</t>
   </si>
   <si>
-    <t>SOE added indicator</t>
+    <t>Nutrient inputs and water quality near shore</t>
+  </si>
+  <si>
+    <t>summary of data from National Estuarine Research Reserve network started, example info included here</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
   <si>
     <t>(McKinney 2010, Kim Hyde also on this paper)</t>
   </si>
   <si>
-    <t>Cold pool index</t>
-  </si>
-  <si>
-    <t>Nutrient inputs and water quality near shore</t>
-  </si>
-  <si>
-    <t>summary of data from National Estuarine Research Reserve network started, example info included here</t>
-  </si>
-  <si>
     <t>Link environmental and social, economic indicators</t>
   </si>
   <si>
+    <t>SOE habitat wind overlap, page 2 conceptual model</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Quantitative overlap of wind area and habitat and fishing areas</t>
+  </si>
+  <si>
+    <t>SOE habitat wind overlap, wind overlap with fisheries for next round</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Include links to Social Science websites</t>
+  </si>
+  <si>
+    <t>SOE link included in both reports</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Management complexity</t>
+  </si>
+  <si>
+    <t>project started by summer student in 2018, needs further analysis</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>South atlantic managed species represented in recreational indices - break out species managed by MA, SA and AS.</t>
+  </si>
+  <si>
+    <t>SOE revised indicator and noted change in report</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Add social elements from overview conceptual model to NE conceptual model</t>
+  </si>
+  <si>
+    <t>older general conceptual model replaced by specific links between indicators in report</t>
+  </si>
+  <si>
     <t>High (Mid)</t>
   </si>
   <si>
-    <t>SOE habitat wind overlap, page 2 conceptual model</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Avg weight of diet components by feeding group</t>
   </si>
   <si>
     <t>NERRs summary started discuss in memo</t>
   </si>
   <si>
-    <t>Quantitative overlap of wind area and habitat and fishing areas</t>
-  </si>
-  <si>
     <t>NERR network? Chesapeake Bay water quality (existing), ECOMON (tried last year, try again?)</t>
   </si>
   <si>
+    <t>stomach fullness analysis started--species level; feedback requested</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
     <t>Also, get from EPA report? Nearshore habitat risk assessment element</t>
   </si>
   <si>
-    <t>SOE habitat wind overlap, wind overlap with fisheries for next round</t>
+    <t>North Atlantic Right Whale calf production indicator</t>
   </si>
   <si>
     <t>Climate/LTL/Habitat and Human dimension</t>
@@ -266,13 +359,37 @@
     <t>Economic and Social LINK TO Habitat Quality and Ecosystem Productivity</t>
   </si>
   <si>
-    <t>Include links to Social Science websites</t>
-  </si>
-  <si>
     <t>HIgh</t>
   </si>
   <si>
-    <t>SOE link included in both reports</t>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Distinguish managed species in report</t>
+  </si>
+  <si>
+    <t>SOE Council managed species separated in landings figures</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Marine Mammal consumption</t>
+  </si>
+  <si>
+    <t>SOE added discussion of seal diets</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Small pelagic abundance</t>
+  </si>
+  <si>
+    <t>SOE have survey planktivore time series but would like to improve; see also SOE forage energy density</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
   <si>
     <t>SOE habitat wind overlap, 2 pager conceptual model</t>
@@ -281,16 +398,25 @@
     <t>Syntheisis</t>
   </si>
   <si>
-    <t>Management complexity</t>
-  </si>
-  <si>
-    <t>project started by summer student in 2018, needs further analysis</t>
-  </si>
-  <si>
-    <t>South atlantic managed species represented in recreational indices - break out species managed by MA, SA and AS.</t>
-  </si>
-  <si>
-    <t>SOE revised indicator and noted change in report</t>
+    <t>Young of Year index from multiple surveys</t>
+  </si>
+  <si>
+    <t>SOE fish production from NEFSC trawl; feedback reqested on how to expand</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Biomass of sharks</t>
+  </si>
+  <si>
+    <t>HMS provided landings for 3 years and working on full time series, still looking for source of biomass data</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Diversity metric for NEFSC trawl survey</t>
   </si>
   <si>
     <t>Kevin habitat occupancy and trends in lease areas, Geret effort in lease areas, BOEM hotspot analyses?</t>
@@ -299,7 +425,13 @@
     <t>MAFMC Risk Assessment need</t>
   </si>
   <si>
-    <t>Add social elements from overview conceptual model to NE conceptual model</t>
+    <t>need to reconcile different survey vessel catchabilites or split by vessel</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Mean stomach weight across feeding guilds</t>
   </si>
   <si>
     <t>Comm + everyone</t>
@@ -308,21 +440,39 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>older general conceptual model replaced by specific links between indicators in report</t>
+    <t>28</t>
   </si>
   <si>
     <t>Report card like alaska</t>
   </si>
   <si>
+    <t>Ecosystem risk score</t>
+  </si>
+  <si>
     <t>SOE 2 pager bullets</t>
   </si>
   <si>
+    <t>SOE PP required a step towards this; feedback requested for other desired analyses</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
     <t>2 pager</t>
   </si>
   <si>
     <t>Top three points! 1.Ecosystem-&gt;fisheries productivity (Focus on LTL - Nutrient imput to fish production MA very interested how to create synthetic narrative), 2. ocean heat waves (currents/setup, impacts)? 3. other ocean uses/wind MA 3. ecosystem and right whales NE?</t>
   </si>
   <si>
+    <t>Inflection points for indicators</t>
+  </si>
+  <si>
+    <t>inadequate resources to do inflection point and threshold analysis this year</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
     <t>Summary visualization</t>
   </si>
   <si>
@@ -335,21 +485,12 @@
     <t>Head of each Report Section, also Summary?</t>
   </si>
   <si>
-    <t>Avg weight of diet components by feeding group</t>
-  </si>
-  <si>
-    <t>stomach fullness analysis started--species level; feedback requested</t>
-  </si>
-  <si>
     <t>Create forum for formal response</t>
   </si>
   <si>
     <t>Changes at request of Councils. What is new/Top 3 points for the section</t>
   </si>
   <si>
-    <t>North Atlantic Right Whale calf production indicator</t>
-  </si>
-  <si>
     <t>Human dimension</t>
   </si>
   <si>
@@ -362,66 +503,30 @@
     <t>SOE NEFMC (add to mid)</t>
   </si>
   <si>
-    <t>Distinguish managed species in report</t>
-  </si>
-  <si>
     <t>did for Council 2019 report</t>
   </si>
   <si>
-    <t>SOE Council managed species separated in landings figures</t>
-  </si>
-  <si>
-    <t>Marine Mammal consumption</t>
-  </si>
-  <si>
     <t>MAFMC Risk Assessment</t>
   </si>
   <si>
-    <t>SOE added discussion of seal diets</t>
-  </si>
-  <si>
     <t>work started by summer student, needs further analysis</t>
   </si>
   <si>
-    <t>Small pelagic abundance</t>
-  </si>
-  <si>
     <t xml:space="preserve">Complete current project </t>
   </si>
   <si>
     <t>Summer student project last year</t>
   </si>
   <si>
-    <t>SOE have survey planktivore time series but would like to improve; see also SOE forage energy density</t>
-  </si>
-  <si>
-    <t>Young of Year index from multiple surveys</t>
-  </si>
-  <si>
-    <t>SOE fish production from NEFSC trawl; feedback reqested on how to expand</t>
-  </si>
-  <si>
     <t>SOE revised rec catch diversity</t>
   </si>
   <si>
-    <t>Biomass of sharks</t>
-  </si>
-  <si>
     <t>SSB to determine</t>
   </si>
   <si>
-    <t>HMS provided landings for 3 years and working on full time series, still looking for source of biomass data</t>
-  </si>
-  <si>
-    <t>Diversity metric for NEFSC trawl survey</t>
-  </si>
-  <si>
     <t>See summary</t>
   </si>
   <si>
-    <t>need to reconcile different survey vessel catchabilites or split by vessel</t>
-  </si>
-  <si>
     <t>older general conceptual model repoaced by specific links between indicators in report</t>
   </si>
   <si>
@@ -431,15 +536,9 @@
     <t>Could just cut and paste from NE Shelf to MA and GOM/GB, but whole infographic may be done over</t>
   </si>
   <si>
-    <t>Mean stomach weight across feeding guilds</t>
-  </si>
-  <si>
     <t>Megafauna</t>
   </si>
   <si>
-    <t>Ecosystem risk score</t>
-  </si>
-  <si>
     <t>stomach fullness analysis started--species level</t>
   </si>
   <si>
@@ -449,19 +548,10 @@
     <t>Bigelow + NEAMAP + longline + seabirds?</t>
   </si>
   <si>
-    <t>SOE PP required a step towards this; feedback requested for other desired analyses</t>
-  </si>
-  <si>
     <t>If jellies show up as fluctuating, could be a place to link abundance time series in</t>
   </si>
   <si>
-    <t>Inflection points for indicators</t>
-  </si>
-  <si>
     <t>Protected Species</t>
-  </si>
-  <si>
-    <t>inadequate resources to do inflection point and threshold analysis this year</t>
   </si>
   <si>
     <t>Contact Chris Orphanides (PSB)</t>
@@ -607,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -622,6 +712,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -863,13 +956,13 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -911,16 +1004,16 @@
     <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>11</v>
@@ -929,375 +1022,375 @@
         <v>20</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>103</v>
+        <v>153</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>104</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>11</v>
@@ -1306,436 +1399,436 @@
         <v>12</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="3" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>113</v>
+        <v>160</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>112</v>
+        <v>159</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="3" t="s">
-        <v>111</v>
+        <v>158</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>136</v>
+        <v>171</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>151</v>
+        <v>181</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>153</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>154</v>
+        <v>184</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>155</v>
+        <v>185</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>122</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>138</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>143</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="3" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="2" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="3" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="5" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="3" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -1775,7 +1868,7 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
@@ -1797,316 +1890,316 @@
       <c r="C3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3">
-        <v>1.0</v>
+      <c r="D3" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.0</v>
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3.0</v>
+        <v>30</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3">
-        <v>4.0</v>
+        <v>35</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="3">
-        <v>5.0</v>
+        <v>41</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="3">
-        <v>6.0</v>
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="3">
-        <v>7.0</v>
+      <c r="C9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="3">
-        <v>8.0</v>
+        <v>28</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="3">
-        <v>9.0</v>
+        <v>65</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="3">
-        <v>10.0</v>
+        <v>69</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="3">
-        <v>11.0</v>
+        <v>75</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="3">
-        <v>12.0</v>
+        <v>75</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="3">
-        <v>13.0</v>
+        <v>83</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="3">
-        <v>14.0</v>
+        <v>87</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="3">
-        <v>15.0</v>
+        <v>90</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="3">
-        <v>16.0</v>
+        <v>28</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="3">
-        <v>17.0</v>
+        <v>96</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="3">
-        <v>18.0</v>
+        <v>99</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="3">
-        <v>19.0</v>
+        <v>102</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D22" s="3">
-        <v>20.0</v>
+        <v>108</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="3">
-        <v>21.0</v>
+        <v>75</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="3">
-        <v>22.0</v>
+      <c r="D24" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="3">
-        <v>23.0</v>
+      <c r="D25" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="26">
@@ -2114,55 +2207,55 @@
         <v>122</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" s="3">
-        <v>24.0</v>
+        <v>123</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D27" s="3">
-        <v>25.0</v>
+        <v>128</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="D28" s="3">
-        <v>26.0</v>
+      <c r="D28" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="3">
-        <v>27.0</v>
+        <v>136</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="30">
@@ -2170,41 +2263,41 @@
         <v>138</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" s="3">
-        <v>28.0</v>
+        <v>108</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="D31" s="3">
-        <v>29.0</v>
+        <v>145</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" s="3">
-        <v>30.0</v>
+        <v>150</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update table with pp required, draft text through 5
</commit_message>
<xml_diff>
--- a/SOE-response-memo/2019requests.xlsx
+++ b/SOE-response-memo/2019requests.xlsx
@@ -29,6 +29,126 @@
     <t>Memo Section</t>
   </si>
   <si>
+    <t>Formal response to requests</t>
+  </si>
+  <si>
+    <t>Both Councils</t>
+  </si>
+  <si>
+    <t>this response memo</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Consider report card like Alaska's</t>
+  </si>
+  <si>
+    <t>SOE summary bullets (page 1)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Include summary visualization</t>
+  </si>
+  <si>
+    <t>SOE infographics (page 2)</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Include uncertainty estimates for all indicators</t>
+  </si>
+  <si>
+    <t>SOE survey biomass uncertainty included; feedback requested for other indicators</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Include Downeast ME (Scotian Shelf EPU)</t>
+  </si>
+  <si>
+    <t>NEFMC</t>
+  </si>
+  <si>
+    <t>SOE survey biomass now includes most; included in other indicators</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Link zooplankton abundance and or community composition to fish condition</t>
+  </si>
+  <si>
+    <t>SOE page 2 research spotlight</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Ocean acidification information</t>
+  </si>
+  <si>
+    <t>inadequate information for indicator; existing info summarized here</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Gulf Stream Index/Labrador current interaction</t>
+  </si>
+  <si>
+    <t>SOE Labrador current and Gulf Stream indices now included in both reports</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Include source for PP estimates (satellite vs in situ)</t>
+  </si>
+  <si>
+    <t>SOE clarified that all PP estimates are from satellite</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Shellfish growth/distribution linked to climate (system productivity)</t>
+  </si>
+  <si>
+    <t>MAFMC</t>
+  </si>
+  <si>
+    <t>project with R. Mann student to start late 2020</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Esturine condition relative to power plants and temp</t>
+  </si>
+  <si>
+    <t>inadequate resourses to address this year</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Frequency and occurance of warm rings</t>
+  </si>
+  <si>
+    <t>SOE added indicator</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Cold pool index</t>
+  </si>
+  <si>
     <t>Working group</t>
   </si>
   <si>
@@ -38,9 +158,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Formal response to requests</t>
-  </si>
-  <si>
     <t>Products/ things to work on</t>
   </si>
   <si>
@@ -50,67 +167,82 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Both Councils</t>
-  </si>
-  <si>
-    <t>this response memo</t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>Consider report card like Alaska's</t>
-  </si>
-  <si>
-    <t>SOE summary bullets (page 1)</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Nutrient inputs and water quality near shore</t>
+  </si>
+  <si>
+    <t>summary of data from National Estuarine Research Reserve network started, example info included here</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Link environmental and social, economic indicators</t>
+  </si>
+  <si>
+    <t>SOE PP required, habitat and wind overlap, page 2 conceptual model</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Quantitative overlap of wind area and habitat and fishing areas</t>
+  </si>
+  <si>
+    <t>SOE habitat wind overlap, wind overlap with fisheries for next round</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
+    <t>Include links to Social Science websites</t>
+  </si>
+  <si>
     <t>Highest</t>
   </si>
   <si>
+    <t>SOE link included in both reports</t>
+  </si>
+  <si>
     <t>Uncertainty estimates for all indicators</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Management complexity</t>
+  </si>
+  <si>
     <t>SOE survey biomass</t>
   </si>
   <si>
     <t>Indicator specific uncertainty estimates</t>
   </si>
   <si>
-    <t>Include summary visualization</t>
-  </si>
-  <si>
-    <t>SOE infographics (page 2)</t>
-  </si>
-  <si>
-    <t>2</t>
+    <t>project started by summer student in 2018, needs further analysis</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>Improve communciation</t>
   </si>
   <si>
-    <t>Include uncertainty estimates for all indicators</t>
-  </si>
-  <si>
-    <t>Include Downeast ME (Scotian Shelf EPU)</t>
-  </si>
-  <si>
-    <t>NEFMC</t>
+    <t>South atlantic managed species represented in recreational indices - break out species managed by MA, SA and AS.</t>
+  </si>
+  <si>
+    <t>SOE revised indicator and noted change in report</t>
   </si>
   <si>
     <t>SOE survey biomass, and many indicators include</t>
   </si>
   <si>
-    <t>SOE survey biomass uncertainty included; feedback requested for other indicators</t>
-  </si>
-  <si>
-    <t>3</t>
+    <t>18</t>
   </si>
   <si>
     <t>Ask Council/SSC</t>
@@ -119,19 +251,22 @@
     <t>include as SS or combined SS and GOM? SSC comment just says to clarify, could continue with current GOM</t>
   </si>
   <si>
+    <t>Add social elements from overview conceptual model to NE conceptual model</t>
+  </si>
+  <si>
+    <t>older general conceptual model replaced by specific links between indicators in report</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>Climate/LTL/Habitat</t>
   </si>
   <si>
-    <t>SOE survey biomass now includes most; included in other indicators</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Habitat Quality and Ecosystem Productivity</t>
   </si>
   <si>
-    <t>Link zooplankton abundance and or community composition to fish condition</t>
+    <t>Avg weight of diet components by feeding group</t>
   </si>
   <si>
     <t>High</t>
@@ -140,100 +275,133 @@
     <t>Link zooplankton abundance and or comunity composition to fish condition</t>
   </si>
   <si>
-    <t>SOE page 2 research spotlight</t>
+    <t>stomach fullness analysis started--species level; feedback requested</t>
+  </si>
+  <si>
+    <t>20</t>
   </si>
   <si>
     <t>SOE 2 pager, explain ongoing research in memo</t>
   </si>
   <si>
-    <t>5</t>
+    <t>North Atlantic Right Whale calf production indicator</t>
   </si>
   <si>
     <t>Synthesize existing indicators</t>
   </si>
   <si>
-    <t>Ocean acidification information</t>
-  </si>
-  <si>
     <t>Add longline survey condition?</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>both already in this section</t>
   </si>
   <si>
-    <t>inadequate information for indicator; existing info summarized here</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>Gulf Stream Index/Labrador current interaction</t>
-  </si>
-  <si>
-    <t>SOE Labrador current and Gulf Stream indices now included in both reports</t>
+    <t>Distinguish managed species in report</t>
+  </si>
+  <si>
+    <t>SOE Council managed species separated in landings figures</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Marine Mammal consumption</t>
   </si>
   <si>
     <t>OA</t>
   </si>
   <si>
+    <t>SOE added discussion of seal diets</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
     <t xml:space="preserve">not enough yet sampling table in memo? </t>
   </si>
   <si>
+    <t>Small pelagic abundance</t>
+  </si>
+  <si>
     <t>At least report on efforts if data are not there yet</t>
   </si>
   <si>
+    <t>SOE have survey planktivore time series but would like to improve; see also SOE forage energy density</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Young of Year index from multiple surveys</t>
+  </si>
+  <si>
+    <t>SOE fish production from NEFSC trawl; feedback reqested on how to expand</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Biomass of sharks</t>
+  </si>
+  <si>
     <t>SOE eco conditoins NEFMC</t>
   </si>
   <si>
+    <t>HMS provided landings for 3 years and working on full time series, still looking for source of biomass data</t>
+  </si>
+  <si>
     <t>Heat wave stuff (Vince)</t>
   </si>
   <si>
+    <t>26</t>
+  </si>
+  <si>
     <t>Already in report, integrate with other indicators?</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Include source for PP estimates (satellite vs in situ)</t>
-  </si>
-  <si>
-    <t>SOE clarified that all PP estiamtes are from satellite</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Shellfish growth/distribution linked to climate (system productivity)</t>
-  </si>
-  <si>
-    <t>MAFMC</t>
+    <t>Diversity metric for NEFSC trawl survey</t>
+  </si>
+  <si>
+    <t>need to reconcile different survey vessel catchabilites or split by vessel</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Mean stomach weight across feeding guilds</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
   <si>
     <t>SOE add to text satellite</t>
   </si>
   <si>
-    <t>project with R. Mann student to start late 2020</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>Ecosystem risk score</t>
   </si>
   <si>
     <t>Easy, just clarify in report</t>
   </si>
   <si>
-    <t>Esturine condition relative to power plants and temp</t>
-  </si>
-  <si>
-    <t>inadequate resourses to address this year</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>SOE PP required a step towards this; feedback requested for other desired analyses</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Inflection points for indicators</t>
   </si>
   <si>
     <t>Fish and Invertebrates LINK TO Habitat Quality and Ecosystem Productivity</t>
   </si>
   <si>
-    <t>Frequency and occurance of warm rings</t>
+    <t>inadequate resources to do inflection point and threshold analysis this year</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>Moderate</t>
@@ -242,117 +410,30 @@
     <t>Shellfish growth'dist linked to climate (system productivity)</t>
   </si>
   <si>
-    <t>SOE added indicator</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>project with R Mann student to start late 2020? in memo</t>
   </si>
   <si>
-    <t>Cold pool index</t>
-  </si>
-  <si>
     <t>(Roger Mann VIMS data Contribution)</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>Economic and Social (new section Other Ocean Uses?)</t>
   </si>
   <si>
-    <t>Nutrient inputs and water quality near shore</t>
-  </si>
-  <si>
-    <t>summary of data from National Estuarine Research Reserve network started, example info included here</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>(McKinney 2010, Kim Hyde also on this paper)</t>
   </si>
   <si>
-    <t>Link environmental and social, economic indicators</t>
-  </si>
-  <si>
-    <t>SOE habitat wind overlap, page 2 conceptual model</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Quantitative overlap of wind area and habitat and fishing areas</t>
-  </si>
-  <si>
-    <t>SOE habitat wind overlap, wind overlap with fisheries for next round</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Include links to Social Science websites</t>
-  </si>
-  <si>
-    <t>SOE link included in both reports</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Management complexity</t>
-  </si>
-  <si>
-    <t>project started by summer student in 2018, needs further analysis</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>South atlantic managed species represented in recreational indices - break out species managed by MA, SA and AS.</t>
-  </si>
-  <si>
-    <t>SOE revised indicator and noted change in report</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Add social elements from overview conceptual model to NE conceptual model</t>
-  </si>
-  <si>
-    <t>older general conceptual model replaced by specific links between indicators in report</t>
-  </si>
-  <si>
     <t>High (Mid)</t>
   </si>
   <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Avg weight of diet components by feeding group</t>
-  </si>
-  <si>
     <t>NERRs summary started discuss in memo</t>
   </si>
   <si>
     <t>NERR network? Chesapeake Bay water quality (existing), ECOMON (tried last year, try again?)</t>
   </si>
   <si>
-    <t>stomach fullness analysis started--species level; feedback requested</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Also, get from EPA report? Nearshore habitat risk assessment element</t>
   </si>
   <si>
-    <t>North Atlantic Right Whale calf production indicator</t>
-  </si>
-  <si>
     <t>Climate/LTL/Habitat and Human dimension</t>
   </si>
   <si>
@@ -362,115 +443,34 @@
     <t>HIgh</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Distinguish managed species in report</t>
-  </si>
-  <si>
-    <t>SOE Council managed species separated in landings figures</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Marine Mammal consumption</t>
-  </si>
-  <si>
-    <t>SOE added discussion of seal diets</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>Small pelagic abundance</t>
-  </si>
-  <si>
-    <t>SOE have survey planktivore time series but would like to improve; see also SOE forage energy density</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>SOE habitat wind overlap, 2 pager conceptual model</t>
   </si>
   <si>
     <t>Syntheisis</t>
   </si>
   <si>
-    <t>Young of Year index from multiple surveys</t>
-  </si>
-  <si>
-    <t>SOE fish production from NEFSC trawl; feedback reqested on how to expand</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Biomass of sharks</t>
-  </si>
-  <si>
-    <t>HMS provided landings for 3 years and working on full time series, still looking for source of biomass data</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Diversity metric for NEFSC trawl survey</t>
-  </si>
-  <si>
     <t>Kevin habitat occupancy and trends in lease areas, Geret effort in lease areas, BOEM hotspot analyses?</t>
   </si>
   <si>
     <t>MAFMC Risk Assessment need</t>
   </si>
   <si>
-    <t>need to reconcile different survey vessel catchabilites or split by vessel</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
-    <t>Mean stomach weight across feeding guilds</t>
-  </si>
-  <si>
     <t>Comm + everyone</t>
   </si>
   <si>
     <t>Summary</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
     <t>Report card like alaska</t>
   </si>
   <si>
-    <t>Ecosystem risk score</t>
-  </si>
-  <si>
     <t>SOE 2 pager bullets</t>
   </si>
   <si>
-    <t>SOE PP required a step towards this; feedback requested for other desired analyses</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
     <t>2 pager</t>
   </si>
   <si>
     <t>Top three points! 1.Ecosystem-&gt;fisheries productivity (Focus on LTL - Nutrient imput to fish production MA very interested how to create synthetic narrative), 2. ocean heat waves (currents/setup, impacts)? 3. other ocean uses/wind MA 3. ecosystem and right whales NE?</t>
-  </si>
-  <si>
-    <t>Inflection points for indicators</t>
-  </si>
-  <si>
-    <t>inadequate resources to do inflection point and threshold analysis this year</t>
-  </si>
-  <si>
-    <t>30</t>
   </si>
   <si>
     <t>Summary visualization</t>
@@ -710,7 +710,6 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -720,6 +719,7 @@
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -956,13 +956,13 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -970,433 +970,433 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>40</v>
+        <v>84</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>42</v>
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>46</v>
+        <v>90</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>55</v>
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>57</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>77</v>
+        <v>34</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>72</v>
+        <v>129</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>75</v>
+        <v>34</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>78</v>
+        <v>129</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>75</v>
+        <v>34</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>86</v>
+        <v>141</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>125</v>
+        <v>18</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>90</v>
+        <v>34</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>144</v>
+        <v>5</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>152</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="3" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>155</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>12</v>
+        <v>5</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>156</v>
@@ -1416,11 +1416,11 @@
       <c r="D18" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>92</v>
+      <c r="E18" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>161</v>
@@ -1438,21 +1438,21 @@
         <v>163</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>164</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="3" t="s">
         <v>166</v>
       </c>
     </row>
@@ -1465,13 +1465,13 @@
         <v>159</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>167</v>
@@ -1485,18 +1485,18 @@
         <v>158</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>101</v>
+      <c r="E21" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>170</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -1512,21 +1512,21 @@
         <v>173</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>105</v>
+        <v>84</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="3" t="s">
         <v>175</v>
       </c>
       <c r="I22" s="3" t="s">
@@ -1544,16 +1544,16 @@
         <v>178</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>75</v>
+        <v>18</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>179</v>
@@ -1570,13 +1570,13 @@
         <v>181</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>116</v>
+        <v>71</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>182</v>
@@ -1594,13 +1594,13 @@
         <v>178</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>184</v>
@@ -1621,13 +1621,13 @@
         <v>187</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>188</v>
@@ -1648,13 +1648,13 @@
         <v>187</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>191</v>
@@ -1675,13 +1675,13 @@
         <v>187</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>194</v>
@@ -1698,13 +1698,13 @@
         <v>187</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>196</v>
@@ -1719,21 +1719,21 @@
         <v>173</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="3" t="s">
         <v>175</v>
       </c>
       <c r="I30" s="3" t="s">
@@ -1746,18 +1746,18 @@
         <v>198</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>143</v>
+        <v>62</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="3" t="s">
         <v>199</v>
       </c>
       <c r="H31" s="3" t="s">
@@ -1773,18 +1773,18 @@
         <v>198</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>202</v>
       </c>
       <c r="H32" s="3" t="s">
@@ -1805,14 +1805,14 @@
         <v>206</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>208</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="3" t="s">
         <v>210</v>
       </c>
     </row>
@@ -1868,436 +1868,436 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="5" t="s">
+    <row r="5">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>36</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="s">
-        <v>38</v>
+      <c r="A7" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>45</v>
+      <c r="A8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>61</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="s">
-        <v>62</v>
+      <c r="A11" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>66</v>
+        <v>34</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>70</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="3" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>76</v>
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>80</v>
+        <v>41</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>84</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>88</v>
+        <v>18</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>91</v>
+        <v>58</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>94</v>
+        <v>18</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>97</v>
+        <v>34</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>100</v>
+        <v>34</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>104</v>
+        <v>18</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>109</v>
+        <v>5</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>115</v>
+        <v>41</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>118</v>
+        <v>18</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>121</v>
+        <v>34</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>124</v>
+        <v>34</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>129</v>
+        <v>34</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>132</v>
+        <v>34</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>137</v>
+        <v>18</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>141</v>
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>146</v>
+        <v>34</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>151</v>
+        <v>5</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PPR figs, update table, text up to 20
</commit_message>
<xml_diff>
--- a/SOE-response-memo/2019requests.xlsx
+++ b/SOE-response-memo/2019requests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="214">
   <si>
     <t>Request</t>
   </si>
@@ -44,12 +44,30 @@
     <t>Consider report card like Alaska's</t>
   </si>
   <si>
+    <t>Working group</t>
+  </si>
+  <si>
+    <t>Report Section</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
     <t>SOE summary bullets (page 1)</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
+    <t>Products/ things to work on</t>
+  </si>
+  <si>
+    <t>New Data opportunities</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>Include summary visualization</t>
   </si>
   <si>
@@ -77,36 +95,66 @@
     <t>SOE survey biomass now includes most; included in other indicators</t>
   </si>
   <si>
+    <t>All</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
     <t>Link zooplankton abundance and or community composition to fish condition</t>
   </si>
   <si>
+    <t>Highest</t>
+  </si>
+  <si>
+    <t>Uncertainty estimates for all indicators</t>
+  </si>
+  <si>
     <t>SOE page 2 research spotlight</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
+    <t>SOE survey biomass</t>
+  </si>
+  <si>
+    <t>Indicator specific uncertainty estimates</t>
+  </si>
+  <si>
     <t>Ocean acidification information</t>
   </si>
   <si>
-    <t>inadequate information for indicator; existing info summarized here</t>
+    <t>work in progress to develop baseline and monitoring</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
+    <t>Improve communciation</t>
+  </si>
+  <si>
     <t>Gulf Stream Index/Labrador current interaction</t>
   </si>
   <si>
     <t>SOE Labrador current and Gulf Stream indices now included in both reports</t>
   </si>
   <si>
+    <t>SOE survey biomass, and many indicators include</t>
+  </si>
+  <si>
+    <t>Ask Council/SSC</t>
+  </si>
+  <si>
+    <t>include as SS or combined SS and GOM? SSC comment just says to clarify, could continue with current GOM</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
+    <t>Climate/LTL/Habitat</t>
+  </si>
+  <si>
     <t>Include source for PP estimates (satellite vs in situ)</t>
   </si>
   <si>
@@ -128,487 +176,445 @@
     <t>9</t>
   </si>
   <si>
+    <t>Habitat Quality and Ecosystem Productivity</t>
+  </si>
+  <si>
+    <t>Estuarine condition relative to power plants and temp</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>inadequate resourses to address this year</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Link zooplankton abundance and or comunity composition to fish condition</t>
+  </si>
+  <si>
+    <t>Frequency and occurrence of warm core rings</t>
+  </si>
+  <si>
+    <t>SOE 2 pager, explain ongoing research in memo</t>
+  </si>
+  <si>
+    <t>SOE added indicator</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Synthesize existing indicators</t>
+  </si>
+  <si>
+    <t>Add longline survey condition?</t>
+  </si>
+  <si>
+    <t>Cold pool index</t>
+  </si>
+  <si>
+    <t>both already in this section</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Nutrient inputs and water quality near shore</t>
+  </si>
+  <si>
+    <t>summary of data from National Estuarine Research Reserve network started, example info included here</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not enough yet sampling table in memo? </t>
+  </si>
+  <si>
+    <t>Link environmental and social, economic indicators</t>
+  </si>
+  <si>
+    <t>At least report on efforts if data are not there yet</t>
+  </si>
+  <si>
+    <t>SOE PP required, habitat and wind overlap, page 2 conceptual model</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Quantitative overlap of wind area and habitat and fishing areas</t>
+  </si>
+  <si>
+    <t>SOE habitat wind overlap, wind overlap with fisheries for next round</t>
+  </si>
+  <si>
+    <t>SOE eco conditoins NEFMC</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Heat wave stuff (Vince)</t>
+  </si>
+  <si>
+    <t>Already in report, integrate with other indicators?</t>
+  </si>
+  <si>
+    <t>Include links to Social Science websites</t>
+  </si>
+  <si>
+    <t>SOE link included in both reports</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Management complexity</t>
+  </si>
+  <si>
+    <t>project started by summer student in 2018, needs further analysis</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>SOE add to text satellite</t>
+  </si>
+  <si>
+    <t>South atlantic managed species represented in recreational indices - break out species managed by MA, SA and AS.</t>
+  </si>
+  <si>
+    <t>Easy, just clarify in report</t>
+  </si>
+  <si>
+    <t>SOE revised indicator and noted change in report</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Add social elements from overview conceptual model to NE conceptual model</t>
+  </si>
+  <si>
+    <t>Fish and Invertebrates LINK TO Habitat Quality and Ecosystem Productivity</t>
+  </si>
+  <si>
+    <t>older general conceptual model replaced by specific links between indicators in report</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Shellfish growth'dist linked to climate (system productivity)</t>
+  </si>
+  <si>
+    <t>Avg weight of diet components by feeding group, mean stomach weight across feeding guilds</t>
+  </si>
+  <si>
+    <t>project with R Mann student to start late 2020? in memo</t>
+  </si>
+  <si>
+    <t>stomach fullness analysis started--species level; feedback requested</t>
+  </si>
+  <si>
+    <t>(Roger Mann VIMS data Contribution)</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>North Atlantic Right Whale calf production indicator</t>
+  </si>
+  <si>
+    <t>Economic and Social (new section Other Ocean Uses?)</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>Esturine condition relative to power plants and temp</t>
   </si>
   <si>
-    <t>inadequate resourses to address this year</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>(McKinney 2010, Kim Hyde also on this paper)</t>
+  </si>
+  <si>
+    <t>Distinguish managed species in report</t>
+  </si>
+  <si>
+    <t>SOE Council managed species separated in landings figures</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Marine Mammal consumption</t>
   </si>
   <si>
     <t>Frequency and occurance of warm rings</t>
   </si>
   <si>
-    <t>SOE added indicator</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>Cold pool index</t>
-  </si>
-  <si>
-    <t>Working group</t>
-  </si>
-  <si>
-    <t>Report Section</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Products/ things to work on</t>
-  </si>
-  <si>
-    <t>New Data opportunities</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Nutrient inputs and water quality near shore</t>
-  </si>
-  <si>
-    <t>summary of data from National Estuarine Research Reserve network started, example info included here</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Link environmental and social, economic indicators</t>
-  </si>
-  <si>
-    <t>SOE PP required, habitat and wind overlap, page 2 conceptual model</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Quantitative overlap of wind area and habitat and fishing areas</t>
-  </si>
-  <si>
-    <t>SOE habitat wind overlap, wind overlap with fisheries for next round</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Include links to Social Science websites</t>
-  </si>
-  <si>
-    <t>Highest</t>
-  </si>
-  <si>
-    <t>SOE link included in both reports</t>
-  </si>
-  <si>
-    <t>Uncertainty estimates for all indicators</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Management complexity</t>
-  </si>
-  <si>
-    <t>SOE survey biomass</t>
-  </si>
-  <si>
-    <t>Indicator specific uncertainty estimates</t>
-  </si>
-  <si>
-    <t>project started by summer student in 2018, needs further analysis</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>Improve communciation</t>
-  </si>
-  <si>
-    <t>South atlantic managed species represented in recreational indices - break out species managed by MA, SA and AS.</t>
-  </si>
-  <si>
-    <t>SOE revised indicator and noted change in report</t>
-  </si>
-  <si>
-    <t>SOE survey biomass, and many indicators include</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>Ask Council/SSC</t>
-  </si>
-  <si>
-    <t>include as SS or combined SS and GOM? SSC comment just says to clarify, could continue with current GOM</t>
-  </si>
-  <si>
-    <t>Add social elements from overview conceptual model to NE conceptual model</t>
-  </si>
-  <si>
-    <t>older general conceptual model replaced by specific links between indicators in report</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Climate/LTL/Habitat</t>
-  </si>
-  <si>
-    <t>Habitat Quality and Ecosystem Productivity</t>
+    <t>SOE added discussion of seal diets</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Small pelagic abundance</t>
+  </si>
+  <si>
+    <t>SOE have survey planktivore time series but would like to improve; see also SOE forage energy density</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Young of Year index from multiple surveys</t>
+  </si>
+  <si>
+    <t>SOE fish production from NEFSC trawl; feedback reqested on how to expand</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>High (Mid)</t>
+  </si>
+  <si>
+    <t>Biomass of sharks</t>
+  </si>
+  <si>
+    <t>HMS provided landings for 3 years and working on full time series, still looking for source of biomass data</t>
+  </si>
+  <si>
+    <t>NERRs summary started discuss in memo</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>NERR network? Chesapeake Bay water quality (existing), ECOMON (tried last year, try again?)</t>
+  </si>
+  <si>
+    <t>Also, get from EPA report? Nearshore habitat risk assessment element</t>
+  </si>
+  <si>
+    <t>Diversity metric for NEFSC trawl survey</t>
+  </si>
+  <si>
+    <t>need to reconcile different survey vessel catchabilites or split by vessel</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>Climate/LTL/Habitat and Human dimension</t>
+  </si>
+  <si>
+    <t>Economic and Social LINK TO Habitat Quality and Ecosystem Productivity</t>
+  </si>
+  <si>
+    <t>HIgh</t>
+  </si>
+  <si>
+    <t>SOE habitat wind overlap, 2 pager conceptual model</t>
+  </si>
+  <si>
+    <t>Ecosystem risk score</t>
+  </si>
+  <si>
+    <t>Syntheisis</t>
+  </si>
+  <si>
+    <t>SOE PP required a step towards this; feedback requested for other desired analyses</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>Inflection points for indicators</t>
+  </si>
+  <si>
+    <t>inadequate resources to do inflection point and threshold analysis this year</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>Kevin habitat occupancy and trends in lease areas, Geret effort in lease areas, BOEM hotspot analyses?</t>
+  </si>
+  <si>
+    <t>MAFMC Risk Assessment need</t>
+  </si>
+  <si>
+    <t>Comm + everyone</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Report card like alaska</t>
+  </si>
+  <si>
+    <t>SOE 2 pager bullets</t>
+  </si>
+  <si>
+    <t>2 pager</t>
+  </si>
+  <si>
+    <t>Top three points! 1.Ecosystem-&gt;fisheries productivity (Focus on LTL - Nutrient imput to fish production MA very interested how to create synthetic narrative), 2. ocean heat waves (currents/setup, impacts)? 3. other ocean uses/wind MA 3. ecosystem and right whales NE?</t>
+  </si>
+  <si>
+    <t>Summary visualization</t>
+  </si>
+  <si>
+    <t>SOE 2 pager graphics</t>
+  </si>
+  <si>
+    <t>Infographic</t>
+  </si>
+  <si>
+    <t>Head of each Report Section, also Summary?</t>
+  </si>
+  <si>
+    <t>Create forum for formal response</t>
+  </si>
+  <si>
+    <t>Changes at request of Councils. What is new/Top 3 points for the section</t>
+  </si>
+  <si>
+    <t>Human dimension</t>
+  </si>
+  <si>
+    <t>Economic and Social</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>SOE NEFMC (add to mid)</t>
+  </si>
+  <si>
+    <t>did for Council 2019 report</t>
+  </si>
+  <si>
+    <t>MAFMC Risk Assessment</t>
+  </si>
+  <si>
+    <t>work started by summer student, needs further analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete current project </t>
+  </si>
+  <si>
+    <t>Summer student project last year</t>
+  </si>
+  <si>
+    <t>SOE revised rec catch diversity</t>
+  </si>
+  <si>
+    <t>SSB to determine</t>
+  </si>
+  <si>
+    <t>See summary</t>
+  </si>
+  <si>
+    <t>older general conceptual model repoaced by specific links between indicators in report</t>
+  </si>
+  <si>
+    <t>Conceptual model update</t>
+  </si>
+  <si>
+    <t>Could just cut and paste from NE Shelf to MA and GOM/GB, but whole infographic may be done over</t>
+  </si>
+  <si>
+    <t>Megafauna</t>
   </si>
   <si>
     <t>Avg weight of diet components by feeding group</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Link zooplankton abundance and or comunity composition to fish condition</t>
-  </si>
-  <si>
-    <t>stomach fullness analysis started--species level; feedback requested</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>SOE 2 pager, explain ongoing research in memo</t>
-  </si>
-  <si>
-    <t>North Atlantic Right Whale calf production indicator</t>
-  </si>
-  <si>
-    <t>Synthesize existing indicators</t>
-  </si>
-  <si>
-    <t>Add longline survey condition?</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>both already in this section</t>
-  </si>
-  <si>
-    <t>Distinguish managed species in report</t>
-  </si>
-  <si>
-    <t>SOE Council managed species separated in landings figures</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>Marine Mammal consumption</t>
-  </si>
-  <si>
-    <t>OA</t>
-  </si>
-  <si>
-    <t>SOE added discussion of seal diets</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not enough yet sampling table in memo? </t>
-  </si>
-  <si>
-    <t>Small pelagic abundance</t>
-  </si>
-  <si>
-    <t>At least report on efforts if data are not there yet</t>
-  </si>
-  <si>
-    <t>SOE have survey planktivore time series but would like to improve; see also SOE forage energy density</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Young of Year index from multiple surveys</t>
-  </si>
-  <si>
-    <t>SOE fish production from NEFSC trawl; feedback reqested on how to expand</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Biomass of sharks</t>
-  </si>
-  <si>
-    <t>SOE eco conditoins NEFMC</t>
-  </si>
-  <si>
-    <t>HMS provided landings for 3 years and working on full time series, still looking for source of biomass data</t>
-  </si>
-  <si>
-    <t>Heat wave stuff (Vince)</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Already in report, integrate with other indicators?</t>
-  </si>
-  <si>
-    <t>Diversity metric for NEFSC trawl survey</t>
-  </si>
-  <si>
-    <t>need to reconcile different survey vessel catchabilites or split by vessel</t>
-  </si>
-  <si>
-    <t>27</t>
+    <t>stomach fullness analysis started--species level</t>
+  </si>
+  <si>
+    <t>Food habits summaries</t>
+  </si>
+  <si>
+    <t>Bigelow + NEAMAP + longline + seabirds?</t>
+  </si>
+  <si>
+    <t>If jellies show up as fluctuating, could be a place to link abundance time series in</t>
+  </si>
+  <si>
+    <t>Protected Species</t>
+  </si>
+  <si>
+    <t>Contact Chris Orphanides (PSB)</t>
+  </si>
+  <si>
+    <t>(Gutbrod et al 2015)</t>
+  </si>
+  <si>
+    <t>Document Orientation; Economic and Social; Fish and Invertebrates</t>
+  </si>
+  <si>
+    <t>SOE council managed species in figs, table</t>
+  </si>
+  <si>
+    <t>Table 2 attempted this; figures separate council managed and all seafood, revenue, and biomass; needs more emphasis?</t>
+  </si>
+  <si>
+    <t>SOE added discussion of seal diets, memo no new consumption ests since Smith et al but could be in the future once work is complete</t>
+  </si>
+  <si>
+    <t>Herring Assessment</t>
+  </si>
+  <si>
+    <t>possibly came from 2012 herring assessment, ask Laurel</t>
+  </si>
+  <si>
+    <t>Fish and Invertebrates</t>
+  </si>
+  <si>
+    <t>SOE have survey planktivore time series but would like to improve</t>
+  </si>
+  <si>
+    <t>Combine herring, mackerel, menhaden, other assessments?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">already include planktivore survey indices; previous index possibly came from ESR as survey index, problematic from assessment standpoint; </t>
+  </si>
+  <si>
+    <t>SOE fish production from NEFSC trawl, want to expand this?</t>
+  </si>
+  <si>
+    <t>Bigelow + NEAMAP + CHESMAP/other state surveys? + seabirds?</t>
+  </si>
+  <si>
+    <t>Evaluate resources to do</t>
+  </si>
+  <si>
+    <t>HMS got us landings for 3 years, need more time to get time series, still looking for source of biomass data</t>
+  </si>
+  <si>
+    <t>HMS assessments</t>
+  </si>
+  <si>
+    <t>still need to reconcile different vessel catchabilites</t>
+  </si>
+  <si>
+    <t>Bigelow + other state surveys?</t>
   </si>
   <si>
     <t>Mean stomach weight across feeding guilds</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>SOE add to text satellite</t>
-  </si>
-  <si>
-    <t>Ecosystem risk score</t>
-  </si>
-  <si>
-    <t>Easy, just clarify in report</t>
-  </si>
-  <si>
-    <t>SOE PP required a step towards this; feedback requested for other desired analyses</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Inflection points for indicators</t>
-  </si>
-  <si>
-    <t>Fish and Invertebrates LINK TO Habitat Quality and Ecosystem Productivity</t>
-  </si>
-  <si>
-    <t>inadequate resources to do inflection point and threshold analysis this year</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>Shellfish growth'dist linked to climate (system productivity)</t>
-  </si>
-  <si>
-    <t>project with R Mann student to start late 2020? in memo</t>
-  </si>
-  <si>
-    <t>(Roger Mann VIMS data Contribution)</t>
-  </si>
-  <si>
-    <t>Economic and Social (new section Other Ocean Uses?)</t>
-  </si>
-  <si>
-    <t>(McKinney 2010, Kim Hyde also on this paper)</t>
-  </si>
-  <si>
-    <t>High (Mid)</t>
-  </si>
-  <si>
-    <t>NERRs summary started discuss in memo</t>
-  </si>
-  <si>
-    <t>NERR network? Chesapeake Bay water quality (existing), ECOMON (tried last year, try again?)</t>
-  </si>
-  <si>
-    <t>Also, get from EPA report? Nearshore habitat risk assessment element</t>
-  </si>
-  <si>
-    <t>Climate/LTL/Habitat and Human dimension</t>
-  </si>
-  <si>
-    <t>Economic and Social LINK TO Habitat Quality and Ecosystem Productivity</t>
-  </si>
-  <si>
-    <t>HIgh</t>
-  </si>
-  <si>
-    <t>SOE habitat wind overlap, 2 pager conceptual model</t>
-  </si>
-  <si>
-    <t>Syntheisis</t>
-  </si>
-  <si>
-    <t>Kevin habitat occupancy and trends in lease areas, Geret effort in lease areas, BOEM hotspot analyses?</t>
-  </si>
-  <si>
-    <t>MAFMC Risk Assessment need</t>
-  </si>
-  <si>
-    <t>Comm + everyone</t>
-  </si>
-  <si>
-    <t>Summary</t>
-  </si>
-  <si>
-    <t>Report card like alaska</t>
-  </si>
-  <si>
-    <t>SOE 2 pager bullets</t>
-  </si>
-  <si>
-    <t>2 pager</t>
-  </si>
-  <si>
-    <t>Top three points! 1.Ecosystem-&gt;fisheries productivity (Focus on LTL - Nutrient imput to fish production MA very interested how to create synthetic narrative), 2. ocean heat waves (currents/setup, impacts)? 3. other ocean uses/wind MA 3. ecosystem and right whales NE?</t>
-  </si>
-  <si>
-    <t>Summary visualization</t>
-  </si>
-  <si>
-    <t>SOE 2 pager graphics</t>
-  </si>
-  <si>
-    <t>Infographic</t>
-  </si>
-  <si>
-    <t>Head of each Report Section, also Summary?</t>
-  </si>
-  <si>
-    <t>Create forum for formal response</t>
-  </si>
-  <si>
-    <t>Changes at request of Councils. What is new/Top 3 points for the section</t>
-  </si>
-  <si>
-    <t>Human dimension</t>
-  </si>
-  <si>
-    <t>Economic and Social</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>SOE NEFMC (add to mid)</t>
-  </si>
-  <si>
-    <t>did for Council 2019 report</t>
-  </si>
-  <si>
-    <t>MAFMC Risk Assessment</t>
-  </si>
-  <si>
-    <t>work started by summer student, needs further analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete current project </t>
-  </si>
-  <si>
-    <t>Summer student project last year</t>
-  </si>
-  <si>
-    <t>SOE revised rec catch diversity</t>
-  </si>
-  <si>
-    <t>SSB to determine</t>
-  </si>
-  <si>
-    <t>See summary</t>
-  </si>
-  <si>
-    <t>older general conceptual model repoaced by specific links between indicators in report</t>
-  </si>
-  <si>
-    <t>Conceptual model update</t>
-  </si>
-  <si>
-    <t>Could just cut and paste from NE Shelf to MA and GOM/GB, but whole infographic may be done over</t>
-  </si>
-  <si>
-    <t>Megafauna</t>
-  </si>
-  <si>
-    <t>stomach fullness analysis started--species level</t>
-  </si>
-  <si>
-    <t>Food habits summaries</t>
-  </si>
-  <si>
-    <t>Bigelow + NEAMAP + longline + seabirds?</t>
-  </si>
-  <si>
-    <t>If jellies show up as fluctuating, could be a place to link abundance time series in</t>
-  </si>
-  <si>
-    <t>Protected Species</t>
-  </si>
-  <si>
-    <t>Contact Chris Orphanides (PSB)</t>
-  </si>
-  <si>
-    <t>(Gutbrod et al 2015)</t>
-  </si>
-  <si>
-    <t>Document Orientation; Economic and Social; Fish and Invertebrates</t>
-  </si>
-  <si>
-    <t>SOE council managed species in figs, table</t>
-  </si>
-  <si>
-    <t>Table 2 attempted this; figures separate council managed and all seafood, revenue, and biomass; needs more emphasis?</t>
-  </si>
-  <si>
-    <t>SOE added discussion of seal diets, memo no new consumption ests since Smith et al but could be in the future once work is complete</t>
-  </si>
-  <si>
-    <t>Herring Assessment</t>
-  </si>
-  <si>
-    <t>possibly came from 2012 herring assessment, ask Laurel</t>
-  </si>
-  <si>
-    <t>Fish and Invertebrates</t>
-  </si>
-  <si>
-    <t>SOE have survey planktivore time series but would like to improve</t>
-  </si>
-  <si>
-    <t>Combine herring, mackerel, menhaden, other assessments?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">already include planktivore survey indices; previous index possibly came from ESR as survey index, problematic from assessment standpoint; </t>
-  </si>
-  <si>
-    <t>SOE fish production from NEFSC trawl, want to expand this?</t>
-  </si>
-  <si>
-    <t>Bigelow + NEAMAP + CHESMAP/other state surveys? + seabirds?</t>
-  </si>
-  <si>
-    <t>Evaluate resources to do</t>
-  </si>
-  <si>
-    <t>HMS got us landings for 3 years, need more time to get time series, still looking for source of biomass data</t>
-  </si>
-  <si>
-    <t>HMS assessments</t>
-  </si>
-  <si>
-    <t>still need to reconcile different vessel catchabilites</t>
-  </si>
-  <si>
-    <t>Bigelow + other state surveys?</t>
   </si>
   <si>
     <t>Thresholds/methods</t>
@@ -716,10 +722,10 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -956,13 +962,13 @@
     <row r="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -974,351 +980,351 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
     </row>
     <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="3" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>134</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>144</v>
@@ -1336,7 +1342,7 @@
         <v>147</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>148</v>
@@ -1363,7 +1369,7 @@
         <v>147</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>152</v>
@@ -1387,7 +1393,7 @@
         <v>155</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>4</v>
@@ -1417,10 +1423,10 @@
         <v>160</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>161</v>
@@ -1438,13 +1444,13 @@
         <v>163</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>164</v>
@@ -1465,13 +1471,13 @@
         <v>159</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>167</v>
@@ -1491,10 +1497,10 @@
         <v>169</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>170</v>
@@ -1512,28 +1518,28 @@
         <v>173</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>83</v>
+        <v>174</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23">
@@ -1541,25 +1547,25 @@
         <v>173</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24">
@@ -1567,22 +1573,22 @@
         <v>173</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25">
@@ -1591,25 +1597,25 @@
         <v>173</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26">
@@ -1618,25 +1624,25 @@
         <v>173</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27">
@@ -1645,25 +1651,25 @@
         <v>173</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
@@ -1672,22 +1678,22 @@
         <v>173</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29">
@@ -1695,22 +1701,22 @@
         <v>173</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
@@ -1719,116 +1725,116 @@
         <v>173</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>118</v>
+        <v>199</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3"/>
       <c r="B31" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>147</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H32" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1888,416 +1894,402 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>28</v>
+      <c r="C9" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>37</v>
+      <c r="A12" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>40</v>
+      <c r="A13" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>63</v>
+        <v>24</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="3" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
-        <v>83</v>
+      <c r="A22" s="4" t="s">
+        <v>100</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>